<commit_message>
Removed Code for OLED
</commit_message>
<xml_diff>
--- a/Connections/Circuit connections.xlsx
+++ b/Connections/Circuit connections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arun7\Desktop\Line Follower\Line-Follower-Bot\Connections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A60895-9781-44A1-A9E4-81BFECEE3DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A643905-5EFB-482D-BB72-499DA371AFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,39 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>CIRCUIT CONNECTIONS</t>
   </si>
   <si>
-    <t>OLED CONNECTIONS</t>
-  </si>
-  <si>
-    <t>OLED PIN</t>
-  </si>
-  <si>
-    <t>NANO PINS</t>
-  </si>
-  <si>
     <t>VCC</t>
   </si>
   <si>
     <t>GND</t>
   </si>
   <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
     <t>5V</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A4</t>
   </si>
   <si>
     <t>IR SENSOR CONNECTIONS</t>
@@ -185,10 +164,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,190 +448,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="64.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed code for Motor testong using L298N
</commit_message>
<xml_diff>
--- a/Connections/Circuit connections.xlsx
+++ b/Connections/Circuit connections.xlsx
@@ -8,31 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arun7\Desktop\Line Follower\Line-Follower-Bot\Connections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A643905-5EFB-482D-BB72-499DA371AFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC5CD4-B549-4A8E-A42E-9CD38BDB69B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>CIRCUIT CONNECTIONS</t>
   </si>
   <si>
-    <t>VCC</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -105,16 +111,40 @@
     <t>IN4</t>
   </si>
   <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>D12</t>
   </si>
   <si>
     <t>D13</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2.</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>ENB</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>Battery 12 V</t>
+  </si>
+  <si>
+    <t>Nano 5V</t>
+  </si>
+  <si>
+    <t>GND from battery and Nano</t>
   </si>
 </sst>
 </file>
@@ -448,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="73" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -469,124 +499,148 @@
     </row>
     <row r="3" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>